<commit_message>
Completed Org for Q1
</commit_message>
<xml_diff>
--- a/Data/ALL_CP Bloom_ Data 2022.xlsx
+++ b/Data/ALL_CP Bloom_ Data 2022.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darre\Documents\R\Data\CR Exps\DATA\R_Data Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DarrenThesis\Darren\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AA527D4-4261-4E5A-9598-BF27F51C2CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528ACE7A-D0DF-4537-AB45-602EDE2F75BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55CD2E6E-E69B-446E-92B4-E4A24C2E0687}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55CD2E6E-E69B-446E-92B4-E4A24C2E0687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UseThis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">(Sheet1!$C$2:$C$34,Sheet1!$C$35:$C$85)</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="32">
   <si>
     <t>Sample</t>
   </si>
@@ -127,6 +128,15 @@
   </si>
   <si>
     <t>% Time clams spent open while in experiment</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>WT</t>
   </si>
 </sst>
 </file>
@@ -6876,8 +6886,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="19690080" y="3297555"/>
-              <a:ext cx="7086600" cy="3175635"/>
+              <a:off x="19600545" y="3434715"/>
+              <a:ext cx="7086600" cy="3042285"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7323,18 +7333,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8288EDC-99D0-4FF4-89A3-7FF6F9E6936F}">
   <dimension ref="A1:Y121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="62" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7371,7 +7381,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -7430,7 +7440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -7489,7 +7499,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -7548,7 +7558,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -7607,7 +7617,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>8</v>
       </c>
@@ -7666,7 +7676,7 @@
         <v>4057</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9</v>
       </c>
@@ -7701,7 +7711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>10</v>
       </c>
@@ -7739,7 +7749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -7777,7 +7787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -7842,7 +7852,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -7917,7 +7927,7 @@
         <v>2.8464704321777767</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -7955,7 +7965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -8030,7 +8040,7 @@
         <v>0.93219320061294286</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -8065,7 +8075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>4</v>
       </c>
@@ -8103,7 +8113,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>9</v>
       </c>
@@ -8159,7 +8169,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>10</v>
       </c>
@@ -8222,7 +8232,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>2</v>
       </c>
@@ -8282,7 +8292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>8</v>
       </c>
@@ -8320,7 +8330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>9</v>
       </c>
@@ -8376,7 +8386,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>10</v>
       </c>
@@ -8414,7 +8424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>7</v>
       </c>
@@ -8452,7 +8462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -8493,7 +8503,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -8549,7 +8559,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>8</v>
       </c>
@@ -8615,7 +8625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>9</v>
       </c>
@@ -8681,7 +8691,7 @@
         <v>2.2782616597915593</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>4</v>
       </c>
@@ -8719,7 +8729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>5</v>
       </c>
@@ -8775,7 +8785,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>7</v>
       </c>
@@ -8813,7 +8823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>8</v>
       </c>
@@ -8851,7 +8861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -8886,7 +8896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -8921,7 +8931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>6</v>
       </c>
@@ -8956,7 +8966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>7</v>
       </c>
@@ -8991,7 +9001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>5</v>
       </c>
@@ -9026,7 +9036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -9061,7 +9071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -9096,7 +9106,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>10</v>
       </c>
@@ -9131,7 +9141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>1</v>
       </c>
@@ -9166,7 +9176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>2</v>
       </c>
@@ -9201,7 +9211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>4</v>
       </c>
@@ -9236,7 +9246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>5</v>
       </c>
@@ -9271,7 +9281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>6</v>
       </c>
@@ -9306,7 +9316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7</v>
       </c>
@@ -9341,7 +9351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>9</v>
       </c>
@@ -9376,7 +9386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>1</v>
       </c>
@@ -9411,7 +9421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2</v>
       </c>
@@ -9446,7 +9456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>3</v>
       </c>
@@ -9481,7 +9491,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>4</v>
       </c>
@@ -9516,7 +9526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>6</v>
       </c>
@@ -9551,7 +9561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>9</v>
       </c>
@@ -9586,7 +9596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -9621,7 +9631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2</v>
       </c>
@@ -9656,7 +9666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>5</v>
       </c>
@@ -9691,7 +9701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>6</v>
       </c>
@@ -9726,7 +9736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>10</v>
       </c>
@@ -9761,7 +9771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>1</v>
       </c>
@@ -9796,7 +9806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -9831,7 +9841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>5</v>
       </c>
@@ -9866,7 +9876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>6</v>
       </c>
@@ -9901,7 +9911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>7</v>
       </c>
@@ -9936,7 +9946,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>8</v>
       </c>
@@ -9971,7 +9981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>9</v>
       </c>
@@ -10006,7 +10016,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>2</v>
       </c>
@@ -10041,7 +10051,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>5</v>
       </c>
@@ -10076,7 +10086,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>7</v>
       </c>
@@ -10111,7 +10121,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>8</v>
       </c>
@@ -10146,7 +10156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>10</v>
       </c>
@@ -10181,7 +10191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>1</v>
       </c>
@@ -10216,7 +10226,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>6</v>
       </c>
@@ -10251,7 +10261,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>7</v>
       </c>
@@ -10286,7 +10296,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>9</v>
       </c>
@@ -10321,7 +10331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -10356,7 +10366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3</v>
       </c>
@@ -10391,7 +10401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4</v>
       </c>
@@ -10426,7 +10436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5</v>
       </c>
@@ -10461,7 +10471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>7</v>
       </c>
@@ -10496,7 +10506,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8</v>
       </c>
@@ -10531,7 +10541,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9</v>
       </c>
@@ -10566,7 +10576,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>10</v>
       </c>
@@ -10601,7 +10611,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -10636,7 +10646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>4</v>
       </c>
@@ -10671,7 +10681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6</v>
       </c>
@@ -10706,7 +10716,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>8</v>
       </c>
@@ -10741,7 +10751,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>10</v>
       </c>
@@ -10776,7 +10786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>1</v>
       </c>
@@ -10808,7 +10818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>3</v>
       </c>
@@ -10840,7 +10850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>4</v>
       </c>
@@ -10872,7 +10882,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>5</v>
       </c>
@@ -10904,7 +10914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>6</v>
       </c>
@@ -10936,7 +10946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>7</v>
       </c>
@@ -10968,7 +10978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>8</v>
       </c>
@@ -11000,7 +11010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>9</v>
       </c>
@@ -11032,7 +11042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>10</v>
       </c>
@@ -11064,7 +11074,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>2</v>
       </c>
@@ -11096,7 +11106,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>3</v>
       </c>
@@ -11128,7 +11138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>5</v>
       </c>
@@ -11160,7 +11170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>6</v>
       </c>
@@ -11192,7 +11202,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>7</v>
       </c>
@@ -11224,7 +11234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>10</v>
       </c>
@@ -11256,7 +11266,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>1</v>
       </c>
@@ -11288,7 +11298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>3</v>
       </c>
@@ -11320,7 +11330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>4</v>
       </c>
@@ -11352,7 +11362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>8</v>
       </c>
@@ -11384,7 +11394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>10</v>
       </c>
@@ -11416,7 +11426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <v>1</v>
       </c>
@@ -11448,7 +11458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>2</v>
       </c>
@@ -11480,7 +11490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>5</v>
       </c>
@@ -11512,7 +11522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>6</v>
       </c>
@@ -11544,7 +11554,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>8</v>
       </c>
@@ -11576,7 +11586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>9</v>
       </c>
@@ -11608,7 +11618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1</v>
       </c>
@@ -11640,7 +11650,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2</v>
       </c>
@@ -11672,7 +11682,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>4</v>
       </c>
@@ -11704,7 +11714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>5</v>
       </c>
@@ -11736,7 +11746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8</v>
       </c>
@@ -11768,7 +11778,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>10</v>
       </c>
@@ -11800,7 +11810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="14">
         <v>3</v>
       </c>
@@ -11832,7 +11842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
         <v>6</v>
       </c>
@@ -11864,7 +11874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <v>7</v>
       </c>
@@ -11896,7 +11906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="14">
         <v>9</v>
       </c>
@@ -11933,4 +11943,1593 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3E843-6FF7-4AA0-BDBA-41871B2D1550}">
+  <dimension ref="A1:C121"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <f>Sheet1!C2</f>
+        <v>250</v>
+      </c>
+      <c r="C2">
+        <f>Sheet1!H2</f>
+        <v>-1.4705664199353707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <f>Sheet1!C3</f>
+        <v>250</v>
+      </c>
+      <c r="C3">
+        <f>Sheet1!H3</f>
+        <v>1.5219287634789986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <f>Sheet1!C4</f>
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <f>Sheet1!H4</f>
+        <v>3.2877961914543159E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <f>Sheet1!C5</f>
+        <v>250</v>
+      </c>
+      <c r="C5">
+        <f>Sheet1!H5</f>
+        <v>-1.1056769315556418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <f>Sheet1!C6</f>
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <f>Sheet1!H6</f>
+        <v>-0.39974922685266878</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <f>Sheet1!C7</f>
+        <v>250</v>
+      </c>
+      <c r="C7">
+        <f>Sheet1!H7</f>
+        <v>0.35965976080122647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <f>Sheet1!C8</f>
+        <v>250</v>
+      </c>
+      <c r="C8">
+        <f>Sheet1!H8</f>
+        <v>2.4829420077280013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <f>Sheet1!C9</f>
+        <v>500</v>
+      </c>
+      <c r="C9">
+        <f>Sheet1!H9</f>
+        <v>6.9787044586097663E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <f>Sheet1!C10</f>
+        <v>500</v>
+      </c>
+      <c r="C10">
+        <f>Sheet1!H10</f>
+        <v>9.9231074129466274E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <f>Sheet1!C11</f>
+        <v>500</v>
+      </c>
+      <c r="C11">
+        <f>Sheet1!H11</f>
+        <v>0.66776576132074228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <f>Sheet1!C12</f>
+        <v>500</v>
+      </c>
+      <c r="C12">
+        <f>Sheet1!H12</f>
+        <v>-2.2920909513645693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <f>Sheet1!C13</f>
+        <v>500</v>
+      </c>
+      <c r="C13">
+        <f>Sheet1!H13</f>
+        <v>-3.0885996318149673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <f>Sheet1!C14</f>
+        <v>750</v>
+      </c>
+      <c r="C14">
+        <f>Sheet1!H14</f>
+        <v>-2.7465169729546055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <f>Sheet1!C15</f>
+        <v>750</v>
+      </c>
+      <c r="C15">
+        <f>Sheet1!H15</f>
+        <v>-1.591653608304165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <f>Sheet1!C16</f>
+        <v>750</v>
+      </c>
+      <c r="C16">
+        <f>Sheet1!H16</f>
+        <v>-6.1785969236770182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <f>Sheet1!C17</f>
+        <v>750</v>
+      </c>
+      <c r="C17">
+        <f>Sheet1!H17</f>
+        <v>-4.5429578600065588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <f>Sheet1!C18</f>
+        <v>4745</v>
+      </c>
+      <c r="C18">
+        <f>Sheet1!H18</f>
+        <v>5.6644080342022081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <f>Sheet1!C19</f>
+        <v>4745</v>
+      </c>
+      <c r="C19">
+        <f>Sheet1!H19</f>
+        <v>1.5151909555074661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <f>Sheet1!C20</f>
+        <v>4745</v>
+      </c>
+      <c r="C20">
+        <f>Sheet1!H20</f>
+        <v>2.5259455789623475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <f>Sheet1!C21</f>
+        <v>4745</v>
+      </c>
+      <c r="C21">
+        <f>Sheet1!H21</f>
+        <v>0.59099364101621721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <f>Sheet1!C22</f>
+        <v>250</v>
+      </c>
+      <c r="C22">
+        <f>Sheet1!H22</f>
+        <v>-10.849312506007823</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <f>Sheet1!C23</f>
+        <v>250</v>
+      </c>
+      <c r="C23">
+        <f>Sheet1!H23</f>
+        <v>-10.026180417829162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <f>Sheet1!C24</f>
+        <v>500</v>
+      </c>
+      <c r="C24">
+        <f>Sheet1!H24</f>
+        <v>4.1638214699849341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <f>Sheet1!C25</f>
+        <v>500</v>
+      </c>
+      <c r="C25">
+        <f>Sheet1!H25</f>
+        <v>11.665441116646994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <f>Sheet1!C26</f>
+        <v>500</v>
+      </c>
+      <c r="C26">
+        <f>Sheet1!H26</f>
+        <v>0.366129336988543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <f>Sheet1!C27</f>
+        <v>750</v>
+      </c>
+      <c r="C27">
+        <f>Sheet1!H27</f>
+        <v>-5.4183433583775829</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <f>Sheet1!C28</f>
+        <v>750</v>
+      </c>
+      <c r="C28">
+        <f>Sheet1!H28</f>
+        <v>-9.3931692795532502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <f>Sheet1!C29</f>
+        <v>750</v>
+      </c>
+      <c r="C29">
+        <f>Sheet1!H29</f>
+        <v>0.69470490766305271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <f>Sheet1!C30</f>
+        <v>750</v>
+      </c>
+      <c r="C30">
+        <f>Sheet1!H30</f>
+        <v>-5.8670887967026868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <f>Sheet1!C31</f>
+        <v>250</v>
+      </c>
+      <c r="C31">
+        <f>Sheet1!H31</f>
+        <v>2.7453748314218931</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f>Sheet1!C32</f>
+        <v>250</v>
+      </c>
+      <c r="C32">
+        <f>Sheet1!H32</f>
+        <v>5.2448117028226191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f>Sheet1!C33</f>
+        <v>250</v>
+      </c>
+      <c r="C33">
+        <f>Sheet1!H33</f>
+        <v>-0.86264982117696709</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <f>Sheet1!C34</f>
+        <v>250</v>
+      </c>
+      <c r="C34">
+        <f>Sheet1!H34</f>
+        <v>0.67207621950673935</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <f>Sheet1!C35</f>
+        <v>500</v>
+      </c>
+      <c r="C35">
+        <f>Sheet1!H35</f>
+        <v>16.865983522372694</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36">
+        <f>Sheet1!C36</f>
+        <v>500</v>
+      </c>
+      <c r="C36">
+        <f>Sheet1!H36</f>
+        <v>20.507246285213444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37">
+        <f>Sheet1!C37</f>
+        <v>500</v>
+      </c>
+      <c r="C37">
+        <f>Sheet1!H37</f>
+        <v>20.995579528457448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <f>Sheet1!C38</f>
+        <v>500</v>
+      </c>
+      <c r="C38">
+        <f>Sheet1!H38</f>
+        <v>7.349570620544978</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <f>Sheet1!C39</f>
+        <v>750</v>
+      </c>
+      <c r="C39">
+        <f>Sheet1!H39</f>
+        <v>-4.5977136060480284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <f>Sheet1!C40</f>
+        <v>750</v>
+      </c>
+      <c r="C40">
+        <f>Sheet1!H40</f>
+        <v>10.801330527685987</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41">
+        <f>Sheet1!C41</f>
+        <v>750</v>
+      </c>
+      <c r="C41">
+        <f>Sheet1!H41</f>
+        <v>0.66427316459877273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <f>Sheet1!C42</f>
+        <v>750</v>
+      </c>
+      <c r="C42">
+        <f>Sheet1!H42</f>
+        <v>3.4396750883780496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43">
+        <f>Sheet1!C43</f>
+        <v>750</v>
+      </c>
+      <c r="C43">
+        <f>Sheet1!H43</f>
+        <v>-0.7063137649125395</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <f>Sheet1!C44</f>
+        <v>750</v>
+      </c>
+      <c r="C44">
+        <f>Sheet1!H44</f>
+        <v>-7.1931760050218827</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45">
+        <f>Sheet1!C45</f>
+        <v>750</v>
+      </c>
+      <c r="C45">
+        <f>Sheet1!H45</f>
+        <v>0.11710403070241594</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46">
+        <f>Sheet1!C46</f>
+        <v>8061</v>
+      </c>
+      <c r="C46">
+        <f>Sheet1!H46</f>
+        <v>0.94802777716523912</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47">
+        <f>Sheet1!C47</f>
+        <v>8061</v>
+      </c>
+      <c r="C47">
+        <f>Sheet1!H47</f>
+        <v>-0.76508085529194558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48">
+        <f>Sheet1!C48</f>
+        <v>8061</v>
+      </c>
+      <c r="C48">
+        <f>Sheet1!H48</f>
+        <v>-4.4936086049767887</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49">
+        <f>Sheet1!C49</f>
+        <v>8061</v>
+      </c>
+      <c r="C49">
+        <f>Sheet1!H49</f>
+        <v>-0.41478881293961761</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50">
+        <f>Sheet1!C50</f>
+        <v>8061</v>
+      </c>
+      <c r="C50">
+        <f>Sheet1!H50</f>
+        <v>0.74296738346810021</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51">
+        <f>Sheet1!C51</f>
+        <v>8061</v>
+      </c>
+      <c r="C51">
+        <f>Sheet1!H51</f>
+        <v>-6.8096145393055432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52">
+        <f>Sheet1!C52</f>
+        <v>250</v>
+      </c>
+      <c r="C52">
+        <f>Sheet1!H52</f>
+        <v>-4.2221028393961539</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <f>Sheet1!C53</f>
+        <v>250</v>
+      </c>
+      <c r="C53">
+        <f>Sheet1!H53</f>
+        <v>-1.1688648473858727</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54">
+        <f>Sheet1!C54</f>
+        <v>250</v>
+      </c>
+      <c r="C54">
+        <f>Sheet1!H54</f>
+        <v>-13.863372788975445</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55">
+        <f>Sheet1!C55</f>
+        <v>250</v>
+      </c>
+      <c r="C55">
+        <f>Sheet1!H55</f>
+        <v>-6.9434158266308357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56">
+        <f>Sheet1!C56</f>
+        <v>250</v>
+      </c>
+      <c r="C56">
+        <f>Sheet1!H56</f>
+        <v>0.4317962080411169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57">
+        <f>Sheet1!C57</f>
+        <v>500</v>
+      </c>
+      <c r="C57">
+        <f>Sheet1!H57</f>
+        <v>2.236168253383759</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58">
+        <f>Sheet1!C58</f>
+        <v>500</v>
+      </c>
+      <c r="C58">
+        <f>Sheet1!H58</f>
+        <v>0.11455947329152959</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59">
+        <f>Sheet1!C59</f>
+        <v>500</v>
+      </c>
+      <c r="C59">
+        <f>Sheet1!H59</f>
+        <v>3.4143334518012787</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60">
+        <f>Sheet1!C60</f>
+        <v>500</v>
+      </c>
+      <c r="C60">
+        <f>Sheet1!H60</f>
+        <v>7.4184796427740682</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61">
+        <f>Sheet1!C61</f>
+        <v>500</v>
+      </c>
+      <c r="C61">
+        <f>Sheet1!H61</f>
+        <v>-2.479658854563743</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62">
+        <f>Sheet1!C62</f>
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <f>Sheet1!H62</f>
+        <v>-3.3391437829240838</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63">
+        <f>Sheet1!C63</f>
+        <v>500</v>
+      </c>
+      <c r="C63">
+        <f>Sheet1!H63</f>
+        <v>2.7260937960606935</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64">
+        <f>Sheet1!C64</f>
+        <v>750</v>
+      </c>
+      <c r="C64">
+        <f>Sheet1!H64</f>
+        <v>-7.2045031580718017</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65">
+        <f>Sheet1!C65</f>
+        <v>750</v>
+      </c>
+      <c r="C65">
+        <f>Sheet1!H65</f>
+        <v>-5.7060650797568648</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66">
+        <f>Sheet1!C66</f>
+        <v>750</v>
+      </c>
+      <c r="C66">
+        <f>Sheet1!H66</f>
+        <v>3.4036124403464552</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67">
+        <f>Sheet1!C67</f>
+        <v>750</v>
+      </c>
+      <c r="C67">
+        <f>Sheet1!H67</f>
+        <v>9.2402692213221655</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68">
+        <f>Sheet1!C68</f>
+        <v>750</v>
+      </c>
+      <c r="C68">
+        <f>Sheet1!H68</f>
+        <v>5.0084526151901034</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69">
+        <f>Sheet1!C69</f>
+        <v>4057</v>
+      </c>
+      <c r="C69">
+        <f>Sheet1!H69</f>
+        <v>0.7992481360258864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70">
+        <f>Sheet1!C70</f>
+        <v>4057</v>
+      </c>
+      <c r="C70">
+        <f>Sheet1!H70</f>
+        <v>2.3150986930400461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71">
+        <f>Sheet1!C71</f>
+        <v>4057</v>
+      </c>
+      <c r="C71">
+        <f>Sheet1!H71</f>
+        <v>1.2164157986436988</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72">
+        <f>Sheet1!C72</f>
+        <v>4057</v>
+      </c>
+      <c r="C72">
+        <f>Sheet1!H72</f>
+        <v>4.7561675324550867</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73">
+        <f>Sheet1!C73</f>
+        <v>3000</v>
+      </c>
+      <c r="C73">
+        <f>Sheet1!H73</f>
+        <v>-3.2221247697570581</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74">
+        <f>Sheet1!C74</f>
+        <v>3000</v>
+      </c>
+      <c r="C74">
+        <f>Sheet1!H74</f>
+        <v>-2.94948350634975</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75">
+        <f>Sheet1!C75</f>
+        <v>3000</v>
+      </c>
+      <c r="C75">
+        <f>Sheet1!H75</f>
+        <v>-6.5551186035597349</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76">
+        <f>Sheet1!C76</f>
+        <v>3000</v>
+      </c>
+      <c r="C76">
+        <f>Sheet1!H76</f>
+        <v>9.9828555504330208</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77">
+        <f>Sheet1!C77</f>
+        <v>3000</v>
+      </c>
+      <c r="C77">
+        <f>Sheet1!H77</f>
+        <v>-0.3822098179350823</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78">
+        <f>Sheet1!C78</f>
+        <v>3000</v>
+      </c>
+      <c r="C78">
+        <f>Sheet1!H78</f>
+        <v>-9.3266274349181693</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79">
+        <f>Sheet1!C79</f>
+        <v>3000</v>
+      </c>
+      <c r="C79">
+        <f>Sheet1!H79</f>
+        <v>16.444726342135002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80">
+        <f>Sheet1!C80</f>
+        <v>3000</v>
+      </c>
+      <c r="C80">
+        <f>Sheet1!H80</f>
+        <v>-4.4544411690807637</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81">
+        <f>Sheet1!C81</f>
+        <v>3000</v>
+      </c>
+      <c r="C81">
+        <f>Sheet1!H81</f>
+        <v>2.4614017729465907</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82">
+        <f>Sheet1!C82</f>
+        <v>3000</v>
+      </c>
+      <c r="C82">
+        <f>Sheet1!H82</f>
+        <v>8.5259528527281603</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83">
+        <f>Sheet1!C83</f>
+        <v>3000</v>
+      </c>
+      <c r="C83">
+        <f>Sheet1!H83</f>
+        <v>7.383955020942885</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84">
+        <f>Sheet1!C84</f>
+        <v>3000</v>
+      </c>
+      <c r="C84">
+        <f>Sheet1!H84</f>
+        <v>11.914697083189818</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85">
+        <f>Sheet1!C85</f>
+        <v>3000</v>
+      </c>
+      <c r="C85">
+        <f>Sheet1!H85</f>
+        <v>-4.7367934943039938</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86">
+        <f>Sheet1!C86</f>
+        <v>250</v>
+      </c>
+      <c r="C86">
+        <f>Sheet1!H86</f>
+        <v>-0.91803990895942555</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87">
+        <f>Sheet1!C87</f>
+        <v>250</v>
+      </c>
+      <c r="C87">
+        <f>Sheet1!H87</f>
+        <v>1.1600432859392658</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88">
+        <f>Sheet1!C88</f>
+        <v>250</v>
+      </c>
+      <c r="C88">
+        <f>Sheet1!H88</f>
+        <v>26.497579210177111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89">
+        <f>Sheet1!C89</f>
+        <v>250</v>
+      </c>
+      <c r="C89">
+        <f>Sheet1!H89</f>
+        <v>4.7940863727742782</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>31</v>
+      </c>
+      <c r="B90">
+        <f>Sheet1!C90</f>
+        <v>250</v>
+      </c>
+      <c r="C90">
+        <f>Sheet1!H90</f>
+        <v>-2.8841497657762747</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91">
+        <f>Sheet1!C91</f>
+        <v>250</v>
+      </c>
+      <c r="C91">
+        <f>Sheet1!H91</f>
+        <v>-4.910608134013942</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>31</v>
+      </c>
+      <c r="B92">
+        <f>Sheet1!C92</f>
+        <v>250</v>
+      </c>
+      <c r="C92">
+        <f>Sheet1!H92</f>
+        <v>-10.207824931003357</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93">
+        <f>Sheet1!C93</f>
+        <v>250</v>
+      </c>
+      <c r="C93">
+        <f>Sheet1!H93</f>
+        <v>8.1334197626678364</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>31</v>
+      </c>
+      <c r="B94">
+        <f>Sheet1!C94</f>
+        <v>250</v>
+      </c>
+      <c r="C94">
+        <f>Sheet1!H94</f>
+        <v>20.877685594336139</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>31</v>
+      </c>
+      <c r="B95">
+        <f>Sheet1!C95</f>
+        <v>750</v>
+      </c>
+      <c r="C95">
+        <f>Sheet1!H95</f>
+        <v>-1.5875676808902146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B96">
+        <f>Sheet1!C96</f>
+        <v>750</v>
+      </c>
+      <c r="C96">
+        <f>Sheet1!H96</f>
+        <v>9.2907530275597328</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97">
+        <f>Sheet1!C97</f>
+        <v>750</v>
+      </c>
+      <c r="C97">
+        <f>Sheet1!H97</f>
+        <v>10.542668520174834</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B98">
+        <f>Sheet1!C98</f>
+        <v>750</v>
+      </c>
+      <c r="C98">
+        <f>Sheet1!H98</f>
+        <v>3.4337252435799552</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>31</v>
+      </c>
+      <c r="B99">
+        <f>Sheet1!C99</f>
+        <v>750</v>
+      </c>
+      <c r="C99">
+        <f>Sheet1!H99</f>
+        <v>-3.4204616271324446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100">
+        <f>Sheet1!C100</f>
+        <v>750</v>
+      </c>
+      <c r="C100">
+        <f>Sheet1!H100</f>
+        <v>12.853470924856245</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>31</v>
+      </c>
+      <c r="B101">
+        <f>Sheet1!C101</f>
+        <v>1000</v>
+      </c>
+      <c r="C101">
+        <f>Sheet1!H101</f>
+        <v>9.8765958985954008</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102">
+        <f>Sheet1!C102</f>
+        <v>1000</v>
+      </c>
+      <c r="C102">
+        <f>Sheet1!H102</f>
+        <v>-8.731495099322041</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103">
+        <f>Sheet1!C103</f>
+        <v>1000</v>
+      </c>
+      <c r="C103">
+        <f>Sheet1!H103</f>
+        <v>-1.0159688959343738</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104">
+        <f>Sheet1!C104</f>
+        <v>1000</v>
+      </c>
+      <c r="C104">
+        <f>Sheet1!H104</f>
+        <v>-9.4902634340213403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105">
+        <f>Sheet1!C105</f>
+        <v>1000</v>
+      </c>
+      <c r="C105">
+        <f>Sheet1!H105</f>
+        <v>1.8490427853198934</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <f>Sheet1!C106</f>
+        <v>9500</v>
+      </c>
+      <c r="C106">
+        <f>Sheet1!H106</f>
+        <v>0.81709636034297639</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>31</v>
+      </c>
+      <c r="B107">
+        <f>Sheet1!C107</f>
+        <v>9500</v>
+      </c>
+      <c r="C107">
+        <f>Sheet1!H107</f>
+        <v>6.8626792930047484</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>31</v>
+      </c>
+      <c r="B108">
+        <f>Sheet1!C108</f>
+        <v>9500</v>
+      </c>
+      <c r="C108">
+        <f>Sheet1!H108</f>
+        <v>1.5902714750929536</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>31</v>
+      </c>
+      <c r="B109">
+        <f>Sheet1!C109</f>
+        <v>9500</v>
+      </c>
+      <c r="C109">
+        <f>Sheet1!H109</f>
+        <v>3.8637140562773906</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110">
+        <f>Sheet1!C110</f>
+        <v>9500</v>
+      </c>
+      <c r="C110">
+        <f>Sheet1!H110</f>
+        <v>3.8292449301048399</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>31</v>
+      </c>
+      <c r="B111">
+        <f>Sheet1!C111</f>
+        <v>9500</v>
+      </c>
+      <c r="C111">
+        <f>Sheet1!H111</f>
+        <v>0.11581647824375535</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112">
+        <f>Sheet1!C112</f>
+        <v>750</v>
+      </c>
+      <c r="C112">
+        <f>Sheet1!H112</f>
+        <v>-0.60122336946268151</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>31</v>
+      </c>
+      <c r="B113">
+        <f>Sheet1!C113</f>
+        <v>750</v>
+      </c>
+      <c r="C113">
+        <f>Sheet1!H113</f>
+        <v>-1.390842274626112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>31</v>
+      </c>
+      <c r="B114">
+        <f>Sheet1!C114</f>
+        <v>750</v>
+      </c>
+      <c r="C114">
+        <f>Sheet1!H114</f>
+        <v>1.3244286438166324</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115">
+        <f>Sheet1!C115</f>
+        <v>750</v>
+      </c>
+      <c r="C115">
+        <f>Sheet1!H115</f>
+        <v>2.7931880751206997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="B116">
+        <f>Sheet1!C116</f>
+        <v>750</v>
+      </c>
+      <c r="C116">
+        <f>Sheet1!H116</f>
+        <v>1.667898402993035</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>31</v>
+      </c>
+      <c r="B117">
+        <f>Sheet1!C117</f>
+        <v>750</v>
+      </c>
+      <c r="C117">
+        <f>Sheet1!H117</f>
+        <v>0.1022317443391193</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>31</v>
+      </c>
+      <c r="B118">
+        <f>Sheet1!C118</f>
+        <v>1500</v>
+      </c>
+      <c r="C118">
+        <f>Sheet1!H118</f>
+        <v>-0.33711366721644631</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>31</v>
+      </c>
+      <c r="B119">
+        <f>Sheet1!C119</f>
+        <v>1500</v>
+      </c>
+      <c r="C119">
+        <f>Sheet1!H119</f>
+        <v>2.9423352028255354</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>31</v>
+      </c>
+      <c r="B120">
+        <f>Sheet1!C120</f>
+        <v>1500</v>
+      </c>
+      <c r="C120">
+        <f>Sheet1!H120</f>
+        <v>2.6207509128800068</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>31</v>
+      </c>
+      <c r="B121">
+        <f>Sheet1!C121</f>
+        <v>1500</v>
+      </c>
+      <c r="C121">
+        <f>Sheet1!H121</f>
+        <v>3.5455386840546499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>